<commit_message>
Traitement des données terminé, passage à la mission 1
</commit_message>
<xml_diff>
--- a/DJU.xlsx
+++ b/DJU.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpaul\Projet_8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFE805DD-85FC-4842-96EE-AECA3F028D2D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC79085B-BB96-4A48-B96E-8B938982E8E1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{2DEA4EBF-5F06-4D82-84C6-FD8F2C33DC85}"/>
   </bookViews>
@@ -222,6 +222,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -251,11 +254,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -573,51 +578,55 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:N1048576"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.90625" style="3"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B1" t="s">
+    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3"/>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2">
+      <c r="A2" s="3">
         <v>2014</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -658,7 +667,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3">
+      <c r="A3" s="3">
         <v>2015</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -699,7 +708,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4">
+      <c r="A4" s="3">
         <v>2016</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -740,7 +749,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A5">
+      <c r="A5" s="3">
         <v>2017</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -781,7 +790,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6">
+      <c r="A6" s="3">
         <v>2018</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -823,5 +832,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>